<commit_message>
oprava cleaningu u žen, nahrání nových dat Mužů, rozdělení notebooku na dvě části, přegnerování vizualizací a ověření s novým PowerBI
</commit_message>
<xml_diff>
--- a/1_zavodnici_W.xlsx
+++ b/1_zavodnici_W.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzelenka\Documents\python_j\fencing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4856DCDE-D226-4735-AF64-87C424805528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10128D4D-A11A-49B6-AE8A-490D5A058FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="-14076" windowWidth="18624" windowHeight="10896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="948" yWindow="-14820" windowWidth="17028" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -976,14 +976,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.77734375" customWidth="1"/>
     <col min="5" max="5" width="18.109375" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>